<commit_message>
uploading issue fixed output file
</commit_message>
<xml_diff>
--- a/secret-santa-2024.xlsx
+++ b/secret-santa-2024.xlsx
@@ -456,12 +456,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Benjamin Collins</t>
+          <t>Matthew King</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>benjamin.collins@acme.com</t>
+          <t>matthew.king.jr@acme.com</t>
         </is>
       </c>
     </row>
@@ -478,12 +478,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hamish Murray</t>
+          <t>Isabella Scott</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>hamish.murray.sr@acme.com</t>
+          <t>isabella.scott@acme.com</t>
         </is>
       </c>
     </row>
@@ -500,12 +500,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hamish Murray</t>
+          <t>Charlie Ross</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>hamish.murray@acme.com</t>
+          <t>charlie.ross.jr@acme.com</t>
         </is>
       </c>
     </row>
@@ -522,12 +522,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Charlie Wright</t>
+          <t>Charlie Ross</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>charlie.wright@acme.com</t>
+          <t>charlie.ross@acme.com</t>
         </is>
       </c>
     </row>
@@ -544,12 +544,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Charlie Ross</t>
+          <t>Piper Stewart</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>charlie.ross.jr@acme.com</t>
+          <t>piper.stewart@acme.com</t>
         </is>
       </c>
     </row>
@@ -566,12 +566,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hamish Murray</t>
+          <t>Charlie Wright</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>hamish.murray.jr@acme.com</t>
+          <t>charlie.wright@acme.com</t>
         </is>
       </c>
     </row>
@@ -588,12 +588,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Layla Graham</t>
+          <t>Matthew King</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>layla.graham@acme.com</t>
+          <t>matthew.king@acme.com</t>
         </is>
       </c>
     </row>
@@ -610,12 +610,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Spencer Allen</t>
+          <t>Benjamin Collins</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>spencer.allen@acme.com</t>
+          <t>benjamin.collins@acme.com</t>
         </is>
       </c>
     </row>
@@ -632,12 +632,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Matthew King</t>
+          <t>Mark Lawrence</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>matthew.king.jr@acme.com</t>
+          <t>mark.lawrence@acme.com</t>
         </is>
       </c>
     </row>
@@ -654,12 +654,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ethan Murray</t>
+          <t>Hamish Murray</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ethan.murray@acme.com</t>
+          <t>hamish.murray.jr@acme.com</t>
         </is>
       </c>
     </row>
@@ -676,12 +676,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Charlie Ross</t>
+          <t>Spencer Allen</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>charlie.ross@acme.com</t>
+          <t>spencer.allen@acme.com</t>
         </is>
       </c>
     </row>
@@ -698,12 +698,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Matthew King</t>
+          <t>Hamish Murray</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>matthew.king@acme.com</t>
+          <t>hamish.murray@acme.com</t>
         </is>
       </c>
     </row>
@@ -720,12 +720,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Isabella Scott</t>
+          <t>Hamish Murray</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>isabella.scott@acme.com</t>
+          <t>hamish.murray.sr@acme.com</t>
         </is>
       </c>
     </row>
@@ -742,12 +742,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Mark Lawrence</t>
+          <t>Ethan Murray</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>mark.lawrence@acme.com</t>
+          <t>ethan.murray@acme.com</t>
         </is>
       </c>
     </row>
@@ -764,12 +764,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Piper Stewart</t>
+          <t>Layla Graham</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>piper.stewart@acme.com</t>
+          <t>layla.graham@acme.com</t>
         </is>
       </c>
     </row>

</xml_diff>